<commit_message>
Anforderungsanalyse erweitert um Prioritätsklassen nach Standard
</commit_message>
<xml_diff>
--- a/SollIstVergleich.xlsx
+++ b/SollIstVergleich.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="16515" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="135" windowWidth="16515" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -533,32 +533,32 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +891,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -905,7 +905,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="28" t="s">
         <v>3</v>
       </c>
@@ -917,7 +917,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="28" t="s">
         <v>4</v>
       </c>
@@ -929,7 +929,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="29" t="s">
@@ -943,7 +943,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="11" t="s">
         <v>55</v>
       </c>
@@ -969,7 +969,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -983,7 +983,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="11" t="s">
         <v>24</v>
       </c>
@@ -995,7 +995,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -1009,7 +1009,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1021,7 +1021,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1035,7 +1035,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="29" t="s">
         <v>17</v>
       </c>
@@ -1047,7 +1047,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -1061,7 +1061,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="20" t="s">
         <v>20</v>
       </c>
@@ -1073,7 +1073,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -1087,7 +1087,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="20" t="s">
         <v>26</v>
       </c>
@@ -1099,7 +1099,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="43" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -1113,7 +1113,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="14" t="s">
         <v>31</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="30" t="s">
         <v>30</v>
       </c>
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
+      <c r="A21" s="45"/>
       <c r="B21" s="13" t="s">
         <v>33</v>
       </c>
@@ -1149,7 +1149,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="13" t="s">
         <v>36</v>
       </c>
@@ -1189,7 +1189,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="32" t="s">
@@ -1203,7 +1203,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="33" t="s">
         <v>41</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
+      <c r="A27" s="45"/>
       <c r="B27" s="34" t="s">
         <v>42</v>
       </c>
@@ -1227,7 +1227,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="43" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="22" t="s">
@@ -1241,7 +1241,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="18" t="s">
         <v>45</v>
       </c>
@@ -1253,7 +1253,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="35" t="s">
         <v>46</v>
       </c>
@@ -1265,7 +1265,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="35" t="s">
         <v>47</v>
       </c>
@@ -1277,7 +1277,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="36" t="s">
         <v>48</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="18" t="s">
         <v>49</v>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="18" t="s">
         <v>61</v>
       </c>
@@ -1313,7 +1313,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="21" t="s">
         <v>50</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="38" t="s">
         <v>62</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="4" t="s">
         <v>63</v>
       </c>
@@ -1368,17 +1368,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A28:A37"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A28:A37"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <conditionalFormatting sqref="D2">
     <cfRule type="iconSet" priority="8">
@@ -1430,7 +1430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -1443,7 +1443,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1451,10 +1451,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="41" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -1462,8 +1462,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="47" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -1471,8 +1471,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="42" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="39" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -1480,7 +1480,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="29" t="s">
@@ -1491,7 +1491,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="11" t="s">
         <v>55</v>
       </c>
@@ -1510,8 +1510,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -1521,8 +1521,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
       <c r="B9" s="11" t="s">
         <v>24</v>
       </c>
@@ -1530,8 +1530,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -1541,8 +1541,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
       <c r="B11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1550,8 +1550,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1561,8 +1561,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
       <c r="B13" s="29" t="s">
         <v>17</v>
       </c>
@@ -1570,8 +1570,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -1581,8 +1581,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="45"/>
       <c r="B15" s="20" t="s">
         <v>20</v>
       </c>
@@ -1590,8 +1590,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -1601,8 +1601,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
       <c r="B17" s="20" t="s">
         <v>26</v>
       </c>
@@ -1611,7 +1611,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="43" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -1621,8 +1621,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="44"/>
       <c r="B19" s="14" t="s">
         <v>31</v>
       </c>
@@ -1630,8 +1630,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="44"/>
       <c r="B20" s="30" t="s">
         <v>30</v>
       </c>
@@ -1639,8 +1639,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="45"/>
       <c r="B21" s="13" t="s">
         <v>33</v>
       </c>
@@ -1649,7 +1649,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -1659,8 +1659,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
       <c r="B23" s="13" t="s">
         <v>36</v>
       </c>
@@ -1679,8 +1679,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="32" t="s">
@@ -1690,8 +1690,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="44"/>
       <c r="B26" s="33" t="s">
         <v>41</v>
       </c>
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
+      <c r="A27" s="45"/>
       <c r="B27" s="34" t="s">
         <v>42</v>
       </c>
@@ -1709,7 +1709,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="43" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="22" t="s">
@@ -1719,8 +1719,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="44"/>
       <c r="B29" s="18" t="s">
         <v>45</v>
       </c>
@@ -1729,7 +1729,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="35" t="s">
         <v>46</v>
       </c>
@@ -1738,7 +1738,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="35" t="s">
         <v>47</v>
       </c>
@@ -1746,8 +1746,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="44"/>
       <c r="B32" s="36" t="s">
         <v>48</v>
       </c>
@@ -1755,8 +1755,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="44"/>
       <c r="B33" s="18" t="s">
         <v>49</v>
       </c>
@@ -1764,8 +1764,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="44"/>
       <c r="B34" s="18" t="s">
         <v>61</v>
       </c>
@@ -1774,7 +1774,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="21" t="s">
         <v>50</v>
       </c>
@@ -1782,8 +1782,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
       <c r="B36" s="38" t="s">
         <v>62</v>
       </c>
@@ -1791,8 +1791,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="45"/>
       <c r="B37" s="4" t="s">
         <v>63</v>
       </c>
@@ -1813,17 +1813,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A28:A37"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>